<commit_message>
add testing ice core data
</commit_message>
<xml_diff>
--- a/data_sample/ice_cores/testing-gap_noextremity-TS.xlsx
+++ b/data_sample/ice_cores/testing-gap_noextremity-TS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -692,7 +692,7 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1281,8 +1281,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>0</v>
+        <v>0.073</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>-9.3</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>-1.9</v>

</xml_diff>